<commit_message>
Mod Tipus Via Dataset
</commit_message>
<xml_diff>
--- a/content/dadesref/entitats/Codis_Territori_TipusVia.xlsx
+++ b/content/dadesref/entitats/Codis_Territori_TipusVia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAA\CTTI\02.Projecte_DadesRef\_____c6\01.CATaleg\07.Proposta_noves_ER\05.OIAD_Paquet_02\06.Tipus_Via\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94981458-2EA9-4EFF-99A5-9B001AF05469}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B87A57-0086-4104-92D1-4BCAB94B3BD0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,7 +937,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -956,6 +956,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1885,10 +1886,10 @@
         <v>218</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>264</v>
+        <v>78</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>266</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1896,10 +1897,10 @@
         <v>219</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1907,10 +1908,10 @@
         <v>220</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1918,10 +1919,10 @@
         <v>221</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1929,10 +1930,10 @@
         <v>222</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1940,10 +1941,10 @@
         <v>223</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1951,10 +1952,10 @@
         <v>224</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1962,7 +1963,7 @@
         <v>225</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>163</v>
+        <v>76</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>75</v>
@@ -1973,10 +1974,10 @@
         <v>226</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1984,10 +1985,10 @@
         <v>227</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1995,10 +1996,10 @@
         <v>228</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -2006,10 +2007,10 @@
         <v>229</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -2017,10 +2018,10 @@
         <v>230</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -2028,10 +2029,10 @@
         <v>231</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -2039,10 +2040,10 @@
         <v>232</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -2050,10 +2051,10 @@
         <v>233</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -2061,10 +2062,10 @@
         <v>234</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -2072,10 +2073,10 @@
         <v>235</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -2083,10 +2084,10 @@
         <v>236</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -2094,10 +2095,10 @@
         <v>237</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -2105,10 +2106,10 @@
         <v>238</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -2116,10 +2117,10 @@
         <v>239</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -2127,10 +2128,10 @@
         <v>240</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -2138,10 +2139,10 @@
         <v>241</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -2149,10 +2150,10 @@
         <v>242</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -2160,10 +2161,10 @@
         <v>243</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -2171,10 +2172,10 @@
         <v>244</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>110</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -2182,10 +2183,10 @@
         <v>245</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>270</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -2193,10 +2194,10 @@
         <v>246</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -2204,10 +2205,10 @@
         <v>247</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -2215,10 +2216,10 @@
         <v>248</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -2226,10 +2227,10 @@
         <v>249</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -2237,10 +2238,10 @@
         <v>250</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -2248,10 +2249,10 @@
         <v>251</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -2259,10 +2260,10 @@
         <v>252</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -2270,10 +2271,10 @@
         <v>253</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -2281,10 +2282,10 @@
         <v>254</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -2292,10 +2293,10 @@
         <v>255</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -2303,10 +2304,10 @@
         <v>256</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -2314,7 +2315,7 @@
         <v>257</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>134</v>
@@ -2325,10 +2326,10 @@
         <v>258</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -2336,10 +2337,10 @@
         <v>259</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -2347,10 +2348,10 @@
         <v>260</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -2358,10 +2359,10 @@
         <v>261</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -2369,21 +2370,21 @@
         <v>262</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>145</v>
+      <c r="B94" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>144</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -2402,7 +2403,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B96:B947 A4:A93 A94:A95" numberStoredAsText="1"/>
+    <ignoredError sqref="B96:B947 A4:A48 A94:A95 A49:A93" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -2411,12 +2412,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2552,18 +2553,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF65D252-1908-44E2-BB35-08282169E652}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6272B2A1-B407-4DF2-A2FE-9044F0D4B8B6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2587,17 +2596,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6272B2A1-B407-4DF2-A2FE-9044F0D4B8B6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF65D252-1908-44E2-BB35-08282169E652}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>